<commit_message>
hobo temp data from Fidalgo Bay
</commit_message>
<xml_diff>
--- a/admin/Histology-Shipment-Info.xlsx
+++ b/admin/Histology-Shipment-Info.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="4">
   <si>
     <t>Histology Casette #</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>Tissue Sample #</t>
+  </si>
+  <si>
+    <t>Shipment on 6/5/2018</t>
   </si>
 </sst>
 </file>
@@ -39,7 +42,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -89,6 +92,27 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -98,7 +122,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -106,8 +130,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -126,8 +165,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -149,8 +216,26 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="18">
+  <cellStyles count="46">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -160,6 +245,20 @@
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -168,6 +267,20 @@
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -497,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G244"/>
+  <dimension ref="A1:G394"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A203" workbookViewId="0">
-      <selection activeCell="H238" sqref="H238"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="E246" sqref="E246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -508,9 +621,8 @@
     <col min="1" max="1" width="10.83203125" style="4"/>
     <col min="2" max="2" width="15.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="6" customWidth="1"/>
-    <col min="4" max="5" width="10.83203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="7" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="10.83203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="7" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
@@ -3389,7 +3501,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="241" spans="1:3">
+    <row r="241" spans="1:7">
       <c r="A241" s="4">
         <f t="shared" si="3"/>
         <v>237</v>
@@ -3401,7 +3513,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="242" spans="1:3">
+    <row r="242" spans="1:7">
       <c r="A242" s="4">
         <f t="shared" si="3"/>
         <v>238</v>
@@ -3413,7 +3525,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="243" spans="1:3">
+    <row r="243" spans="1:7">
       <c r="A243" s="4">
         <f t="shared" si="3"/>
         <v>239</v>
@@ -3425,7 +3537,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="244" spans="1:3">
+    <row r="244" spans="1:7">
       <c r="A244" s="4">
         <f t="shared" si="3"/>
         <v>240</v>
@@ -3437,12 +3549,1512 @@
         <v>72</v>
       </c>
     </row>
+    <row r="245" spans="1:7">
+      <c r="B245" s="5"/>
+    </row>
+    <row r="246" spans="1:7" ht="18">
+      <c r="A246" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B246" s="9"/>
+      <c r="C246" s="10"/>
+    </row>
+    <row r="247" spans="1:7" ht="36">
+      <c r="A247" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B247" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C247" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E247" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F247" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G247" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" ht="18">
+      <c r="A248" s="9">
+        <v>241</v>
+      </c>
+      <c r="B248" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C248" s="10">
+        <v>82</v>
+      </c>
+      <c r="E248" s="9">
+        <v>314</v>
+      </c>
+      <c r="F248" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G248" s="10">
+        <v>95.364788290484896</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" ht="18">
+      <c r="A249" s="9">
+        <v>242</v>
+      </c>
+      <c r="B249" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C249" s="10">
+        <v>82</v>
+      </c>
+      <c r="E249" s="9">
+        <v>315</v>
+      </c>
+      <c r="F249" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G249" s="10">
+        <v>95.524508858874199</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" ht="18">
+      <c r="A250" s="9">
+        <v>243</v>
+      </c>
+      <c r="B250" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C250" s="10">
+        <v>82</v>
+      </c>
+      <c r="E250" s="9">
+        <v>316</v>
+      </c>
+      <c r="F250" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G250" s="10">
+        <v>95.684229427263503</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" ht="18">
+      <c r="A251" s="9">
+        <v>244</v>
+      </c>
+      <c r="B251" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C251" s="10">
+        <v>82</v>
+      </c>
+      <c r="E251" s="9">
+        <v>317</v>
+      </c>
+      <c r="F251" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G251" s="10">
+        <v>95.843949995652807</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" ht="18">
+      <c r="A252" s="9">
+        <v>245</v>
+      </c>
+      <c r="B252" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C252" s="10">
+        <v>82</v>
+      </c>
+      <c r="E252" s="9">
+        <v>318</v>
+      </c>
+      <c r="F252" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G252" s="10">
+        <v>96.003670564042096</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" ht="18">
+      <c r="A253" s="9">
+        <v>246</v>
+      </c>
+      <c r="B253" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C253" s="10">
+        <v>83</v>
+      </c>
+      <c r="E253" s="9">
+        <v>319</v>
+      </c>
+      <c r="F253" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G253" s="10">
+        <v>96.1633911324314</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" ht="18">
+      <c r="A254" s="9">
+        <v>247</v>
+      </c>
+      <c r="B254" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C254" s="10">
+        <v>83</v>
+      </c>
+      <c r="E254" s="9">
+        <v>320</v>
+      </c>
+      <c r="F254" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G254" s="10">
+        <v>96.323111700820704</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" ht="18">
+      <c r="A255" s="9">
+        <v>248</v>
+      </c>
+      <c r="B255" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C255" s="10">
+        <v>83</v>
+      </c>
+      <c r="E255" s="9">
+        <v>321</v>
+      </c>
+      <c r="F255" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G255" s="10">
+        <v>96.642552837599297</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" ht="18">
+      <c r="A256" s="9">
+        <v>249</v>
+      </c>
+      <c r="B256" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C256" s="10">
+        <v>83</v>
+      </c>
+      <c r="E256" s="9">
+        <v>322</v>
+      </c>
+      <c r="F256" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G256" s="10">
+        <v>96.802273405988601</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" ht="18">
+      <c r="A257" s="9">
+        <v>250</v>
+      </c>
+      <c r="B257" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C257" s="10">
+        <v>83</v>
+      </c>
+      <c r="E257" s="9">
+        <v>323</v>
+      </c>
+      <c r="F257" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G257" s="10">
+        <v>96.961993974377904</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" ht="18">
+      <c r="A258" s="9">
+        <v>251</v>
+      </c>
+      <c r="B258" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C258" s="10">
+        <v>84</v>
+      </c>
+      <c r="E258" s="9">
+        <v>324</v>
+      </c>
+      <c r="F258" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G258" s="10">
+        <v>97.121714542767194</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" ht="18">
+      <c r="A259" s="9">
+        <v>252</v>
+      </c>
+      <c r="B259" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C259" s="10">
+        <v>84</v>
+      </c>
+      <c r="E259" s="9">
+        <v>325</v>
+      </c>
+      <c r="F259" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G259" s="10">
+        <v>97.281435111156497</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" ht="18">
+      <c r="A260" s="9">
+        <v>253</v>
+      </c>
+      <c r="B260" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C260" s="10">
+        <v>84</v>
+      </c>
+      <c r="E260" s="9">
+        <v>326</v>
+      </c>
+      <c r="F260" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G260" s="10">
+        <v>97.441155679545801</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" ht="18">
+      <c r="A261" s="9">
+        <v>254</v>
+      </c>
+      <c r="B261" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C261" s="10">
+        <v>84</v>
+      </c>
+      <c r="E261" s="9">
+        <v>327</v>
+      </c>
+      <c r="F261" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G261" s="10">
+        <v>97.600876247935105</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" ht="18">
+      <c r="A262" s="9">
+        <v>255</v>
+      </c>
+      <c r="B262" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C262" s="10">
+        <v>84</v>
+      </c>
+      <c r="E262" s="9">
+        <v>328</v>
+      </c>
+      <c r="F262" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G262" s="10">
+        <v>97.760596816324394</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" ht="18">
+      <c r="A263" s="9">
+        <v>256</v>
+      </c>
+      <c r="B263" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C263" s="10">
+        <v>84.6813186813187</v>
+      </c>
+      <c r="E263" s="9">
+        <v>329</v>
+      </c>
+      <c r="F263" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G263" s="10">
+        <v>97.920317384713698</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" ht="18">
+      <c r="A264" s="9">
+        <v>257</v>
+      </c>
+      <c r="B264" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C264" s="10">
+        <v>84.879120879120904</v>
+      </c>
+      <c r="E264" s="9">
+        <v>330</v>
+      </c>
+      <c r="F264" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G264" s="10">
+        <v>98.080037953103002</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" ht="18">
+      <c r="A265" s="9">
+        <v>258</v>
+      </c>
+      <c r="B265" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C265" s="10">
+        <v>85.076923076923094</v>
+      </c>
+      <c r="E265" s="9">
+        <v>331</v>
+      </c>
+      <c r="F265" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G265" s="10">
+        <v>98.239758521492305</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" ht="18">
+      <c r="A266" s="9">
+        <v>259</v>
+      </c>
+      <c r="B266" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C266" s="10">
+        <v>85.274725274725299</v>
+      </c>
+      <c r="E266" s="9">
+        <v>332</v>
+      </c>
+      <c r="F266" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G266" s="10">
+        <v>98.399479089881595</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" ht="18">
+      <c r="A267" s="9">
+        <v>260</v>
+      </c>
+      <c r="B267" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C267" s="10">
+        <v>85.472527472527503</v>
+      </c>
+      <c r="E267" s="9">
+        <v>333</v>
+      </c>
+      <c r="F267" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G267" s="10">
+        <v>98.559199658270899</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" ht="18">
+      <c r="A268" s="9">
+        <v>261</v>
+      </c>
+      <c r="B268" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C268" s="10">
+        <v>85.670329670329707</v>
+      </c>
+      <c r="E268" s="9">
+        <v>334</v>
+      </c>
+      <c r="F268" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G268" s="10">
+        <v>98.718920226660202</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" ht="18">
+      <c r="A269" s="9">
+        <v>262</v>
+      </c>
+      <c r="B269" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C269" s="10">
+        <v>85.868131868131897</v>
+      </c>
+      <c r="E269" s="9">
+        <v>335</v>
+      </c>
+      <c r="F269" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G269" s="10">
+        <v>98.878640795049506</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" ht="18">
+      <c r="A270" s="9">
+        <v>263</v>
+      </c>
+      <c r="B270" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C270" s="10">
+        <v>86.065934065934101</v>
+      </c>
+      <c r="E270" s="9">
+        <v>336</v>
+      </c>
+      <c r="F270" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G270" s="10">
+        <v>99.038361363438796</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" ht="18">
+      <c r="A271" s="9">
+        <v>264</v>
+      </c>
+      <c r="B271" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C271" s="10">
+        <v>86.263736263736305</v>
+      </c>
+      <c r="E271" s="9">
+        <v>337</v>
+      </c>
+      <c r="F271" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G271" s="10">
+        <v>99.198081931828099</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" ht="18">
+      <c r="A272" s="9">
+        <v>265</v>
+      </c>
+      <c r="B272" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C272" s="10">
+        <v>86.461538461538495</v>
+      </c>
+      <c r="E272" s="9">
+        <v>338</v>
+      </c>
+      <c r="F272" s="13">
+        <v>43172</v>
+      </c>
+      <c r="G272" s="10">
+        <v>99.357802500217403</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" ht="18">
+      <c r="A273" s="9">
+        <v>266</v>
+      </c>
+      <c r="B273" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C273" s="10">
+        <v>86.6593406593407</v>
+      </c>
+      <c r="E273" s="9">
+        <v>339</v>
+      </c>
+      <c r="F273" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G273" s="10">
+        <v>99.517523068606707</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" ht="18">
+      <c r="A274" s="9">
+        <v>267</v>
+      </c>
+      <c r="B274" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C274" s="10">
+        <v>86.857142857142904</v>
+      </c>
+      <c r="E274" s="9">
+        <v>340</v>
+      </c>
+      <c r="F274" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G274" s="10">
+        <v>99.677243636995996</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" ht="18">
+      <c r="A275" s="9">
+        <v>268</v>
+      </c>
+      <c r="B275" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C275" s="10">
+        <v>87.054945054945094</v>
+      </c>
+      <c r="E275" s="9">
+        <v>341</v>
+      </c>
+      <c r="F275" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G275" s="10">
+        <v>99.8369642053853</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" ht="18">
+      <c r="A276" s="9">
+        <v>269</v>
+      </c>
+      <c r="B276" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C276" s="10">
+        <v>87.252747252747298</v>
+      </c>
+      <c r="E276" s="9">
+        <v>342</v>
+      </c>
+      <c r="F276" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G276" s="10">
+        <v>99.996684773774604</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" ht="18">
+      <c r="A277" s="9">
+        <v>270</v>
+      </c>
+      <c r="B277" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C277" s="10">
+        <v>87.450549450549502</v>
+      </c>
+      <c r="E277" s="9">
+        <v>343</v>
+      </c>
+      <c r="F277" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G277" s="10">
+        <v>100.15640534216401</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" ht="18">
+      <c r="A278" s="9">
+        <v>271</v>
+      </c>
+      <c r="B278" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C278" s="10">
+        <v>87.648351648351607</v>
+      </c>
+      <c r="E278" s="9">
+        <v>344</v>
+      </c>
+      <c r="F278" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G278" s="10">
+        <v>100.316125910553</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" ht="18">
+      <c r="A279" s="9">
+        <v>272</v>
+      </c>
+      <c r="B279" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C279" s="10">
+        <v>87.846153846153896</v>
+      </c>
+      <c r="E279" s="9">
+        <v>345</v>
+      </c>
+      <c r="F279" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G279" s="10">
+        <v>100.475846478942</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" ht="18">
+      <c r="A280" s="9">
+        <v>273</v>
+      </c>
+      <c r="B280" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C280" s="10">
+        <v>88.043956043956101</v>
+      </c>
+      <c r="E280" s="9">
+        <v>346</v>
+      </c>
+      <c r="F280" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G280" s="10">
+        <v>100.635567047332</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" ht="18">
+      <c r="A281" s="9">
+        <v>274</v>
+      </c>
+      <c r="B281" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C281" s="10">
+        <v>88.241758241758205</v>
+      </c>
+      <c r="E281" s="9">
+        <v>347</v>
+      </c>
+      <c r="F281" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G281" s="10">
+        <v>100.79528761572099</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" ht="18">
+      <c r="A282" s="9">
+        <v>275</v>
+      </c>
+      <c r="B282" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C282" s="10">
+        <v>88.439560439560495</v>
+      </c>
+      <c r="E282" s="9">
+        <v>348</v>
+      </c>
+      <c r="F282" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G282" s="10">
+        <v>100.95500818411</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" ht="18">
+      <c r="A283" s="9">
+        <v>276</v>
+      </c>
+      <c r="B283" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C283" s="10">
+        <v>88.6373626373626</v>
+      </c>
+      <c r="E283" s="9">
+        <v>349</v>
+      </c>
+      <c r="F283" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G283" s="10">
+        <v>101.1147287525</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" ht="18">
+      <c r="A284" s="9">
+        <v>277</v>
+      </c>
+      <c r="B284" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C284" s="10">
+        <v>88.835164835164804</v>
+      </c>
+      <c r="E284" s="9">
+        <v>350</v>
+      </c>
+      <c r="F284" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G284" s="10">
+        <v>101.274449320889</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" ht="18">
+      <c r="A285" s="9">
+        <v>278</v>
+      </c>
+      <c r="B285" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C285" s="10">
+        <v>89.032967032966994</v>
+      </c>
+      <c r="E285" s="9">
+        <v>351</v>
+      </c>
+      <c r="F285" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G285" s="10">
+        <v>101.434169889278</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" ht="18">
+      <c r="A286" s="9">
+        <v>279</v>
+      </c>
+      <c r="B286" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C286" s="10">
+        <v>89.230769230769198</v>
+      </c>
+      <c r="E286" s="9">
+        <v>352</v>
+      </c>
+      <c r="F286" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G286" s="10">
+        <v>101.593890457667</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" ht="18">
+      <c r="A287" s="9">
+        <v>280</v>
+      </c>
+      <c r="B287" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C287" s="10">
+        <v>89.428571428571402</v>
+      </c>
+      <c r="E287" s="9">
+        <v>353</v>
+      </c>
+      <c r="F287" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G287" s="10">
+        <v>101.753611026057</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" ht="18">
+      <c r="A288" s="9">
+        <v>281</v>
+      </c>
+      <c r="B288" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C288" s="10">
+        <v>89.626373626373606</v>
+      </c>
+      <c r="E288" s="9">
+        <v>354</v>
+      </c>
+      <c r="F288" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G288" s="10">
+        <v>101.91333159444601</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" ht="18">
+      <c r="A289" s="9">
+        <v>282</v>
+      </c>
+      <c r="B289" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C289" s="10">
+        <v>89.824175824175796</v>
+      </c>
+      <c r="E289" s="9">
+        <v>355</v>
+      </c>
+      <c r="F289" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G289" s="10">
+        <v>102.073052162835</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" ht="18">
+      <c r="A290" s="9">
+        <v>283</v>
+      </c>
+      <c r="B290" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C290" s="10">
+        <v>90.021978021978001</v>
+      </c>
+      <c r="E290" s="9">
+        <v>356</v>
+      </c>
+      <c r="F290" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G290" s="10">
+        <v>102.232772731225</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" ht="18">
+      <c r="A291" s="9">
+        <v>284</v>
+      </c>
+      <c r="B291" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C291" s="10">
+        <v>90.219780219780205</v>
+      </c>
+      <c r="E291" s="9">
+        <v>357</v>
+      </c>
+      <c r="F291" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G291" s="10">
+        <v>102.392493299614</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" ht="18">
+      <c r="A292" s="9">
+        <v>285</v>
+      </c>
+      <c r="B292" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C292" s="10">
+        <v>90.417582417582395</v>
+      </c>
+      <c r="E292" s="9">
+        <v>358</v>
+      </c>
+      <c r="F292" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G292" s="10">
+        <v>102.55221386800299</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" ht="18">
+      <c r="A293" s="9">
+        <v>286</v>
+      </c>
+      <c r="B293" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C293" s="10">
+        <v>90.615384615384599</v>
+      </c>
+      <c r="E293" s="9">
+        <v>359</v>
+      </c>
+      <c r="F293" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G293" s="10">
+        <v>102.711934436392</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" ht="18">
+      <c r="A294" s="9">
+        <v>287</v>
+      </c>
+      <c r="B294" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C294" s="10">
+        <v>90.813186813186803</v>
+      </c>
+      <c r="E294" s="9">
+        <v>360</v>
+      </c>
+      <c r="F294" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G294" s="10">
+        <v>102.871655004782</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" ht="18">
+      <c r="A295" s="9">
+        <v>288</v>
+      </c>
+      <c r="B295" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C295" s="10">
+        <v>91.010989010988993</v>
+      </c>
+      <c r="E295" s="9">
+        <v>361</v>
+      </c>
+      <c r="F295" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G295" s="10">
+        <v>103.031375573171</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" ht="18">
+      <c r="A296" s="9">
+        <v>289</v>
+      </c>
+      <c r="B296" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C296" s="10">
+        <v>91.208791208791197</v>
+      </c>
+      <c r="E296" s="9">
+        <v>362</v>
+      </c>
+      <c r="F296" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G296" s="10">
+        <v>103.19109614156</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" ht="18">
+      <c r="A297" s="9">
+        <v>290</v>
+      </c>
+      <c r="B297" s="13">
+        <v>43158</v>
+      </c>
+      <c r="C297" s="10">
+        <v>91.406593406593402</v>
+      </c>
+      <c r="E297" s="9">
+        <v>363</v>
+      </c>
+      <c r="F297" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G297" s="10">
+        <v>103.35081670995</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" ht="18">
+      <c r="A298" s="9">
+        <v>291</v>
+      </c>
+      <c r="B298" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C298" s="10">
+        <v>91.604395604395606</v>
+      </c>
+      <c r="E298" s="9">
+        <v>364</v>
+      </c>
+      <c r="F298" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G298" s="10">
+        <v>103.510537278339</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" ht="18">
+      <c r="A299" s="9">
+        <v>292</v>
+      </c>
+      <c r="B299" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C299" s="10">
+        <v>91.802197802197796</v>
+      </c>
+      <c r="E299" s="9">
+        <v>365</v>
+      </c>
+      <c r="F299" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G299" s="10">
+        <v>103.67025784672801</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" ht="18">
+      <c r="A300" s="9">
+        <v>293</v>
+      </c>
+      <c r="B300" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C300" s="10">
+        <v>92</v>
+      </c>
+      <c r="E300" s="9">
+        <v>366</v>
+      </c>
+      <c r="F300" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G300" s="10">
+        <v>103.82997841511801</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" ht="18">
+      <c r="A301" s="9">
+        <v>294</v>
+      </c>
+      <c r="B301" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C301" s="10">
+        <v>92.197802197802204</v>
+      </c>
+      <c r="E301" s="9">
+        <v>367</v>
+      </c>
+      <c r="F301" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G301" s="10">
+        <v>103.989698983507</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" ht="18">
+      <c r="A302" s="9">
+        <v>295</v>
+      </c>
+      <c r="B302" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C302" s="10">
+        <v>92.395604395604394</v>
+      </c>
+      <c r="E302" s="9">
+        <v>368</v>
+      </c>
+      <c r="F302" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G302" s="10">
+        <v>104.149419551896</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" ht="18">
+      <c r="A303" s="9">
+        <v>296</v>
+      </c>
+      <c r="B303" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C303" s="10">
+        <v>92</v>
+      </c>
+      <c r="E303" s="9">
+        <v>369</v>
+      </c>
+      <c r="F303" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G303" s="10">
+        <v>104.30914012028499</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" ht="18">
+      <c r="A304" s="9">
+        <v>297</v>
+      </c>
+      <c r="B304" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C304" s="10">
+        <v>92.791208791208803</v>
+      </c>
+      <c r="E304" s="9">
+        <v>370</v>
+      </c>
+      <c r="F304" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G304" s="10">
+        <v>104.46886068867499</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" ht="18">
+      <c r="A305" s="9">
+        <v>298</v>
+      </c>
+      <c r="B305" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C305" s="10">
+        <v>92.989010989011007</v>
+      </c>
+      <c r="E305" s="9">
+        <v>371</v>
+      </c>
+      <c r="F305" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G305" s="10">
+        <v>104.628581257064</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" ht="18">
+      <c r="A306" s="9">
+        <v>299</v>
+      </c>
+      <c r="B306" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C306" s="10">
+        <v>93.186813186813197</v>
+      </c>
+      <c r="E306" s="9">
+        <v>372</v>
+      </c>
+      <c r="F306" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G306" s="10">
+        <v>104.788301825453</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" ht="18">
+      <c r="A307" s="9">
+        <v>300</v>
+      </c>
+      <c r="B307" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C307" s="10">
+        <v>93.384615384615401</v>
+      </c>
+      <c r="E307" s="9">
+        <v>373</v>
+      </c>
+      <c r="F307" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G307" s="10">
+        <v>104.948022393843</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" ht="18">
+      <c r="A308" s="9">
+        <v>301</v>
+      </c>
+      <c r="B308" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C308" s="10">
+        <v>93</v>
+      </c>
+      <c r="E308" s="9">
+        <v>374</v>
+      </c>
+      <c r="F308" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G308" s="10">
+        <v>105.107742962232</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" ht="18">
+      <c r="A309" s="9">
+        <v>302</v>
+      </c>
+      <c r="B309" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C309" s="10">
+        <v>93</v>
+      </c>
+      <c r="E309" s="9">
+        <v>375</v>
+      </c>
+      <c r="F309" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G309" s="10">
+        <v>105.267463530621</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" ht="18">
+      <c r="A310" s="9">
+        <v>303</v>
+      </c>
+      <c r="B310" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C310" s="10">
+        <v>93.978021978021999</v>
+      </c>
+      <c r="E310" s="9">
+        <v>376</v>
+      </c>
+      <c r="F310" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G310" s="10">
+        <v>105.42718409901001</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" ht="18">
+      <c r="A311" s="9">
+        <v>304</v>
+      </c>
+      <c r="B311" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C311" s="10">
+        <v>94.175824175824204</v>
+      </c>
+      <c r="E311" s="9">
+        <v>377</v>
+      </c>
+      <c r="F311" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G311" s="10">
+        <v>105.58690466740001</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" ht="18">
+      <c r="A312" s="9">
+        <v>305</v>
+      </c>
+      <c r="B312" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C312" s="10">
+        <v>94.373626373626394</v>
+      </c>
+      <c r="E312" s="9">
+        <v>378</v>
+      </c>
+      <c r="F312" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G312" s="10">
+        <v>105.746625235789</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" ht="18">
+      <c r="A313" s="9">
+        <v>306</v>
+      </c>
+      <c r="B313" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C313" s="10">
+        <v>94</v>
+      </c>
+      <c r="E313" s="9">
+        <v>379</v>
+      </c>
+      <c r="F313" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G313" s="10">
+        <v>105.906345804178</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" ht="18">
+      <c r="A314" s="9">
+        <v>307</v>
+      </c>
+      <c r="B314" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C314" s="10">
+        <v>94</v>
+      </c>
+      <c r="E314" s="9">
+        <v>380</v>
+      </c>
+      <c r="F314" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G314" s="10">
+        <v>106.066066372568</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" ht="18">
+      <c r="A315" s="9">
+        <v>308</v>
+      </c>
+      <c r="B315" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C315" s="10">
+        <v>94</v>
+      </c>
+      <c r="E315" s="9">
+        <v>381</v>
+      </c>
+      <c r="F315" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G315" s="10">
+        <v>106.22578694095699</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" ht="18">
+      <c r="A316" s="9">
+        <v>309</v>
+      </c>
+      <c r="B316" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C316" s="10">
+        <v>94.566185448538405</v>
+      </c>
+      <c r="E316" s="9">
+        <v>382</v>
+      </c>
+      <c r="F316" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G316" s="10">
+        <v>106.385507509346</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" ht="18">
+      <c r="A317" s="9">
+        <v>310</v>
+      </c>
+      <c r="B317" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C317" s="10">
+        <v>94.725906016927695</v>
+      </c>
+      <c r="E317" s="9">
+        <v>383</v>
+      </c>
+      <c r="F317" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G317" s="10">
+        <v>106.545228077735</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" ht="18">
+      <c r="A318" s="9">
+        <v>311</v>
+      </c>
+      <c r="B318" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C318" s="10">
+        <v>94.885626585316999</v>
+      </c>
+      <c r="E318" s="9">
+        <v>384</v>
+      </c>
+      <c r="F318" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G318" s="10">
+        <v>106.704948646125</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" ht="18">
+      <c r="A319" s="9">
+        <v>312</v>
+      </c>
+      <c r="B319" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C319" s="10">
+        <v>95.045347153706302</v>
+      </c>
+      <c r="E319" s="9">
+        <v>385</v>
+      </c>
+      <c r="F319" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G319" s="10">
+        <v>106.864669214514</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" ht="18">
+      <c r="A320" s="9">
+        <v>313</v>
+      </c>
+      <c r="B320" s="13">
+        <v>43172</v>
+      </c>
+      <c r="C320" s="10">
+        <v>95.205067722095606</v>
+      </c>
+      <c r="E320" s="9">
+        <v>386</v>
+      </c>
+      <c r="F320" s="13">
+        <v>43182</v>
+      </c>
+      <c r="G320" s="10">
+        <v>107.024389782903</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" ht="18">
+      <c r="A394" s="9"/>
+      <c r="B394" s="9"/>
+      <c r="C394" s="10"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="69" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="47" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <rowBreaks count="3" manualBreakCount="3">
+    <brk id="197" max="16383" man="1"/>
+    <brk id="245" max="16383" man="1"/>
+    <brk id="394" max="16383" man="1"/>
+  </rowBreaks>
   <colBreaks count="1" manualBreakCount="1">
-    <brk id="3" max="1048575" man="1"/>
+    <brk id="7" max="1048575" man="1"/>
   </colBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>